<commit_message>
20251211 All done except FRD4P
</commit_message>
<xml_diff>
--- a/GUI + Reviews/202509/CAC Family.xlsx
+++ b/GUI + Reviews/202509/CAC Family.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="29029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="5" rupBuild="27928"/>
   <workbookPr defaultThemeVersion="124226"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="V:\PM-Indices-IndexOperations\Review Files\202509\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://euronext-my.sharepoint.com/personal/csonneveld_euronext_com/Documents/Documents/Projects/GUI + Reviews/202509/"/>
     </mc:Choice>
   </mc:AlternateContent>
   <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5550C424-8508-41F7-81C9-B347FEC2BEB0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-29115" yWindow="-16005" windowWidth="29040" windowHeight="15720" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="PX1" sheetId="2" r:id="rId1"/>
@@ -1774,8 +1774,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:F42"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A20" sqref="A20"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F24" sqref="F24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="10.5" x14ac:dyDescent="0.15"/>
@@ -3102,8 +3102,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:F62"/>
   <sheetViews>
-    <sheetView topLeftCell="A3" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:F62"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="10.5" x14ac:dyDescent="0.15"/>

</xml_diff>